<commit_message>
I changed the strain names for RAN12 and RAN13 to Chris Doering's strain names. This is because I wanted to make sure R would recognize that my replicates are for the same strain that Chris' replicates are for and combine them in the "multiple beta-gal" R program. I changed RAN12 to CRD39 and RAN13 to CRD38. However, I'm conducting all the biological replicates for RAN11. Thus, there is no need to change the strain name to Chris Doering's strain name in my R table.
</commit_message>
<xml_diff>
--- a/myData/RAN 7-24-18 BETA GAL RAN11, RAN12, RAN13.xlsx
+++ b/myData/RAN 7-24-18 BETA GAL RAN11, RAN12, RAN13.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TimeCourseAndBetaGalAssays2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2B5CE0-0B77-4EE2-B1DD-1E26E20AD8D1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC2BB53-E883-477B-AB5A-869C8573652A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="22992" windowHeight="13860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,13 +381,13 @@
     <t>RAN11</t>
   </si>
   <si>
-    <t>RAN12</t>
-  </si>
-  <si>
-    <t>RAN13</t>
-  </si>
-  <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>CRD39</t>
+  </si>
+  <si>
+    <t>CRD38</t>
   </si>
 </sst>
 </file>
@@ -3127,7 +3127,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3221,16 +3221,16 @@
         <v>117</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P2" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -3259,16 +3259,16 @@
         <v>117</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -3297,16 +3297,16 @@
         <v>117</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P4" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -3335,16 +3335,16 @@
         <v>117</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P5" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -3866,7 +3866,7 @@
         <v>116</v>
       </c>
       <c r="L18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -3904,7 +3904,7 @@
         <v>116</v>
       </c>
       <c r="L19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -3942,7 +3942,7 @@
         <v>116</v>
       </c>
       <c r="L20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -3980,7 +3980,7 @@
         <v>116</v>
       </c>
       <c r="L21" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -4028,7 +4028,7 @@
         <v>116</v>
       </c>
       <c r="L22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M22">
         <v>26</v>
@@ -4066,7 +4066,7 @@
         <v>116</v>
       </c>
       <c r="L23" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M23">
         <v>26</v>
@@ -4104,7 +4104,7 @@
         <v>116</v>
       </c>
       <c r="L24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M24">
         <v>26</v>
@@ -4142,7 +4142,7 @@
         <v>116</v>
       </c>
       <c r="L25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M25">
         <v>26</v>
@@ -4190,7 +4190,7 @@
         <v>116</v>
       </c>
       <c r="L26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M26">
         <v>89</v>
@@ -4228,7 +4228,7 @@
         <v>116</v>
       </c>
       <c r="L27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M27">
         <v>89</v>
@@ -4266,7 +4266,7 @@
         <v>116</v>
       </c>
       <c r="L28" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M28">
         <v>89</v>
@@ -4304,7 +4304,7 @@
         <v>116</v>
       </c>
       <c r="L29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M29">
         <v>89</v>
@@ -4352,7 +4352,7 @@
         <v>116</v>
       </c>
       <c r="L30" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -4390,7 +4390,7 @@
         <v>116</v>
       </c>
       <c r="L31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M31">
         <v>0</v>
@@ -4428,7 +4428,7 @@
         <v>116</v>
       </c>
       <c r="L32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -4466,7 +4466,7 @@
         <v>116</v>
       </c>
       <c r="L33" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -4514,7 +4514,7 @@
         <v>116</v>
       </c>
       <c r="L34" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M34">
         <v>26</v>
@@ -4552,7 +4552,7 @@
         <v>116</v>
       </c>
       <c r="L35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M35">
         <v>26</v>
@@ -4590,7 +4590,7 @@
         <v>116</v>
       </c>
       <c r="L36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M36">
         <v>26</v>
@@ -4628,7 +4628,7 @@
         <v>116</v>
       </c>
       <c r="L37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M37">
         <v>26</v>
@@ -4676,7 +4676,7 @@
         <v>116</v>
       </c>
       <c r="L38" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M38">
         <v>89</v>
@@ -4714,7 +4714,7 @@
         <v>116</v>
       </c>
       <c r="L39" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M39">
         <v>89</v>
@@ -4752,7 +4752,7 @@
         <v>116</v>
       </c>
       <c r="L40" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M40">
         <v>89</v>
@@ -4790,7 +4790,7 @@
         <v>116</v>
       </c>
       <c r="L41" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M41">
         <v>89</v>
@@ -4816,7 +4816,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4901,7 +4901,7 @@
         <v>117</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N2">
         <v>10</v>
@@ -4933,7 +4933,7 @@
         <v>117</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N3">
         <v>10</v>
@@ -4965,7 +4965,7 @@
         <v>117</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N4">
         <v>10</v>
@@ -4997,7 +4997,7 @@
         <v>117</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N5">
         <v>10</v>
@@ -5450,7 +5450,7 @@
         <v>116</v>
       </c>
       <c r="L18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -5482,7 +5482,7 @@
         <v>116</v>
       </c>
       <c r="L19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -5514,7 +5514,7 @@
         <v>116</v>
       </c>
       <c r="L20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -5546,7 +5546,7 @@
         <v>116</v>
       </c>
       <c r="L21" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -5588,7 +5588,7 @@
         <v>116</v>
       </c>
       <c r="L22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M22">
         <v>26</v>
@@ -5620,7 +5620,7 @@
         <v>116</v>
       </c>
       <c r="L23" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M23">
         <v>26</v>
@@ -5652,7 +5652,7 @@
         <v>116</v>
       </c>
       <c r="L24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M24">
         <v>26</v>
@@ -5684,7 +5684,7 @@
         <v>116</v>
       </c>
       <c r="L25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M25">
         <v>26</v>
@@ -5726,7 +5726,7 @@
         <v>116</v>
       </c>
       <c r="L26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M26">
         <v>89</v>
@@ -5758,7 +5758,7 @@
         <v>116</v>
       </c>
       <c r="L27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M27">
         <v>89</v>
@@ -5790,7 +5790,7 @@
         <v>116</v>
       </c>
       <c r="L28" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M28">
         <v>89</v>
@@ -5822,7 +5822,7 @@
         <v>116</v>
       </c>
       <c r="L29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M29">
         <v>89</v>
@@ -5864,7 +5864,7 @@
         <v>116</v>
       </c>
       <c r="L30" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -5896,7 +5896,7 @@
         <v>116</v>
       </c>
       <c r="L31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M31">
         <v>0</v>
@@ -5928,7 +5928,7 @@
         <v>116</v>
       </c>
       <c r="L32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -5960,7 +5960,7 @@
         <v>116</v>
       </c>
       <c r="L33" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -6002,7 +6002,7 @@
         <v>116</v>
       </c>
       <c r="L34" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M34">
         <v>26</v>
@@ -6034,7 +6034,7 @@
         <v>116</v>
       </c>
       <c r="L35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M35">
         <v>26</v>
@@ -6066,7 +6066,7 @@
         <v>116</v>
       </c>
       <c r="L36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M36">
         <v>26</v>
@@ -6098,7 +6098,7 @@
         <v>116</v>
       </c>
       <c r="L37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M37">
         <v>26</v>
@@ -6140,7 +6140,7 @@
         <v>116</v>
       </c>
       <c r="L38" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M38">
         <v>89</v>
@@ -6172,7 +6172,7 @@
         <v>116</v>
       </c>
       <c r="L39" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M39">
         <v>89</v>
@@ -6204,7 +6204,7 @@
         <v>116</v>
       </c>
       <c r="L40" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M40">
         <v>89</v>
@@ -6236,7 +6236,7 @@
         <v>116</v>
       </c>
       <c r="L41" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M41">
         <v>89</v>

</xml_diff>

<commit_message>
This commit contains 5 replicates of the full osmY promoter (RAN11), 8 replicates of the full astC promoter (CRD39), and 7 replicates of the full gadB promoter. the "analysis of multiple beta-gal experiments" is not calculating the sensitivities of the data and we are working on fixing this. This is only happening to the data sets from "myData/RAN...". I also edited my code to include Chris Doering's code that allows us to view one strain at a time for both the "analysis of a single beta-gal experiment" and "analysis of multiple beta-gal experiments".
</commit_message>
<xml_diff>
--- a/myData/RAN 7-24-18 BETA GAL RAN11, RAN12, RAN13.xlsx
+++ b/myData/RAN 7-24-18 BETA GAL RAN11, RAN12, RAN13.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TimeCourseAndBetaGalAssays2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\royam\Documents\RpoSResearch\betaGal-analysis\myData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC2BB53-E883-477B-AB5A-869C8573652A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6CF3C6-5169-4E85-BCC4-D10D3ABF1E9F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="22992" windowHeight="13860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="122">
   <si>
     <t>A</t>
   </si>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:I103"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3126,8 +3126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4813,1435 +4813,1372 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2">
+      <c r="C1" s="2">
         <v>600</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E1" s="2" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="I1" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="J1" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="N1" s="17" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13" t="s">
         <v>67</v>
       </c>
+      <c r="C2" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
       <c r="D2" s="13">
-        <v>4.2999999999999997E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="E2" s="13">
-        <v>1E-3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2" s="13">
         <v>0</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D3" s="13">
         <v>0</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="13">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="E3" s="13">
-        <v>0</v>
-      </c>
+      <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="I3" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" t="s">
         <v>117</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="L3" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="N3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="13" t="s">
         <v>70</v>
       </c>
+      <c r="C4" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
       <c r="D4" s="13">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="E4" s="13">
         <v>0</v>
       </c>
+      <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="I4" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" t="s">
         <v>117</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="L4" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="N4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="13" t="s">
         <v>71</v>
       </c>
+      <c r="C5" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
       <c r="D5" s="13">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="E5" s="13">
         <v>0</v>
       </c>
+      <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="I5" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" t="s">
         <v>117</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="L5" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="N5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13" t="s">
+      <c r="M5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13" t="s">
         <v>72</v>
       </c>
+      <c r="C6" s="13">
+        <v>0.21</v>
+      </c>
       <c r="D6" s="13">
-        <v>0.21</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="E6" s="13">
-        <v>0.16700000000000001</v>
+        <v>4</v>
       </c>
       <c r="F6" s="13">
-        <v>4</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G6" s="13">
-        <v>0.16300000000000001</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="H6" s="13">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="I6" s="13">
         <v>11.358000000000001</v>
       </c>
-      <c r="J6" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="I6" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" t="s">
         <v>118</v>
       </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
       <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="13" t="s">
         <v>73</v>
       </c>
+      <c r="C7" s="13">
+        <v>0.22</v>
+      </c>
       <c r="D7" s="13">
-        <v>0.22</v>
-      </c>
-      <c r="E7" s="13">
         <v>0.17699999999999999</v>
       </c>
+      <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="I7" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" t="s">
         <v>118</v>
       </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
       <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="13" t="s">
         <v>74</v>
       </c>
+      <c r="C8" s="13">
+        <v>0.214</v>
+      </c>
       <c r="D8" s="13">
-        <v>0.214</v>
-      </c>
-      <c r="E8" s="13">
         <v>0.17100000000000001</v>
       </c>
+      <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="I8" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" t="s">
         <v>118</v>
       </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
       <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="13" t="s">
         <v>75</v>
       </c>
+      <c r="C9" s="13">
+        <v>0.17899999999999999</v>
+      </c>
       <c r="D9" s="13">
-        <v>0.17899999999999999</v>
-      </c>
-      <c r="E9" s="13">
         <v>0.13600000000000001</v>
       </c>
+      <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="I9" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" t="s">
         <v>118</v>
       </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
       <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.157</v>
+      </c>
+      <c r="E10" s="13">
+        <v>4</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="G10" s="13">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H10" s="13">
+        <v>4.7960000000000003</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K10" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10">
         <v>26</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="13">
+      <c r="M10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="13">
         <v>0.2</v>
       </c>
-      <c r="E10" s="13">
+      <c r="D11" s="13">
         <v>0.157</v>
       </c>
-      <c r="F10" s="13">
-        <v>4</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="H10" s="13">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I10" s="13">
-        <v>4.7960000000000003</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L10" t="s">
-        <v>118</v>
-      </c>
-      <c r="M10">
-        <v>26</v>
-      </c>
-      <c r="N10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0.157</v>
-      </c>
+      <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="I11" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K11" t="s">
         <v>118</v>
       </c>
+      <c r="L11">
+        <v>26</v>
+      </c>
       <c r="M11">
-        <v>26</v>
-      </c>
-      <c r="N11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="13" t="s">
         <v>78</v>
       </c>
+      <c r="C12" s="13">
+        <v>0.216</v>
+      </c>
       <c r="D12" s="13">
-        <v>0.216</v>
-      </c>
-      <c r="E12" s="13">
         <v>0.17299999999999999</v>
       </c>
+      <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="I12" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K12" t="s">
         <v>118</v>
       </c>
+      <c r="L12">
+        <v>26</v>
+      </c>
       <c r="M12">
-        <v>26</v>
-      </c>
-      <c r="N12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="13" t="s">
         <v>79</v>
       </c>
+      <c r="C13" s="13">
+        <v>0.20899999999999999</v>
+      </c>
       <c r="D13" s="13">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="E13" s="13">
         <v>0.16600000000000001</v>
       </c>
+      <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="I13" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" t="s">
         <v>118</v>
       </c>
+      <c r="L13">
+        <v>26</v>
+      </c>
       <c r="M13">
-        <v>26</v>
-      </c>
-      <c r="N13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13" t="s">
         <v>80</v>
       </c>
+      <c r="C14" s="13">
+        <v>0.20399999999999999</v>
+      </c>
       <c r="D14" s="13">
-        <v>0.20399999999999999</v>
+        <v>0.161</v>
       </c>
       <c r="E14" s="13">
-        <v>0.161</v>
+        <v>4</v>
       </c>
       <c r="F14" s="13">
-        <v>4</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G14" s="13">
-        <v>0.17799999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H14" s="13">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I14" s="13">
         <v>7.17</v>
       </c>
-      <c r="J14" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="I14" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K14" t="s">
         <v>118</v>
       </c>
+      <c r="L14">
+        <v>89</v>
+      </c>
       <c r="M14">
-        <v>89</v>
-      </c>
-      <c r="N14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="13" t="s">
         <v>81</v>
       </c>
+      <c r="C15" s="13">
+        <v>0.223</v>
+      </c>
       <c r="D15" s="13">
-        <v>0.223</v>
-      </c>
-      <c r="E15" s="13">
         <v>0.18</v>
       </c>
+      <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="I15" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" t="s">
         <v>118</v>
       </c>
+      <c r="L15">
+        <v>89</v>
+      </c>
       <c r="M15">
-        <v>89</v>
-      </c>
-      <c r="N15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="13" t="s">
         <v>82</v>
       </c>
+      <c r="C16" s="13">
+        <v>0.222</v>
+      </c>
       <c r="D16" s="13">
-        <v>0.222</v>
-      </c>
-      <c r="E16" s="13">
         <v>0.17899999999999999</v>
       </c>
+      <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="I16" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" t="s">
         <v>118</v>
       </c>
+      <c r="L16">
+        <v>89</v>
+      </c>
       <c r="M16">
-        <v>89</v>
-      </c>
-      <c r="N16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="13" t="s">
         <v>83</v>
       </c>
+      <c r="C17" s="13">
+        <v>0.23499999999999999</v>
+      </c>
       <c r="D17" s="13">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="E17" s="13">
         <v>0.192</v>
       </c>
+      <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="I17" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K17" t="s">
         <v>118</v>
       </c>
+      <c r="L17">
+        <v>89</v>
+      </c>
       <c r="M17">
-        <v>89</v>
-      </c>
-      <c r="N17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13" t="s">
         <v>84</v>
       </c>
+      <c r="C18" s="13">
+        <v>0.23799999999999999</v>
+      </c>
       <c r="D18" s="13">
-        <v>0.23799999999999999</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="E18" s="13">
-        <v>0.19500000000000001</v>
+        <v>4</v>
       </c>
       <c r="F18" s="13">
-        <v>4</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="G18" s="13">
-        <v>0.20699999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H18" s="13">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I18" s="13">
         <v>6.06</v>
       </c>
-      <c r="J18" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K18" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="I18" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" t="s">
         <v>120</v>
       </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
       <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="13" t="s">
         <v>85</v>
       </c>
+      <c r="C19" s="13">
+        <v>0.26200000000000001</v>
+      </c>
       <c r="D19" s="13">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="E19" s="13">
         <v>0.219</v>
       </c>
+      <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="I19" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K19" t="s">
         <v>120</v>
       </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
       <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="C20" s="13">
+        <v>0.26</v>
+      </c>
       <c r="D20" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="E20" s="13">
         <v>0.217</v>
       </c>
+      <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="I20" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K20" t="s">
         <v>120</v>
       </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
       <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="13" t="s">
         <v>87</v>
       </c>
+      <c r="C21" s="13">
+        <v>0.24099999999999999</v>
+      </c>
       <c r="D21" s="13">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="E21" s="13">
         <v>0.19800000000000001</v>
       </c>
+      <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="I21" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K21" t="s">
         <v>120</v>
       </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
       <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13" t="s">
         <v>88</v>
       </c>
+      <c r="C22" s="13">
+        <v>0.23300000000000001</v>
+      </c>
       <c r="D22" s="13">
-        <v>0.23300000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="E22" s="13">
-        <v>0.19</v>
+        <v>4</v>
       </c>
       <c r="F22" s="13">
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="G22" s="13">
-        <v>0.2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="H22" s="13">
-        <v>2.7E-2</v>
-      </c>
-      <c r="I22" s="13">
         <v>13.507999999999999</v>
       </c>
-      <c r="J22" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="I22" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" t="s">
         <v>120</v>
       </c>
+      <c r="L22">
+        <v>26</v>
+      </c>
       <c r="M22">
-        <v>26</v>
-      </c>
-      <c r="N22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="13" t="s">
         <v>89</v>
       </c>
+      <c r="C23" s="13">
+        <v>0.27200000000000002</v>
+      </c>
       <c r="D23" s="13">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="E23" s="13">
         <v>0.22900000000000001</v>
       </c>
+      <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="I23" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K23" t="s">
         <v>120</v>
       </c>
+      <c r="L23">
+        <v>26</v>
+      </c>
       <c r="M23">
-        <v>26</v>
-      </c>
-      <c r="N23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="13" t="s">
         <v>90</v>
       </c>
+      <c r="C24" s="13">
+        <v>0.21</v>
+      </c>
       <c r="D24" s="13">
-        <v>0.21</v>
-      </c>
-      <c r="E24" s="13">
         <v>0.16700000000000001</v>
       </c>
+      <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="I24" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K24" t="s">
         <v>120</v>
       </c>
+      <c r="L24">
+        <v>26</v>
+      </c>
       <c r="M24">
-        <v>26</v>
-      </c>
-      <c r="N24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="13" t="s">
         <v>91</v>
       </c>
+      <c r="C25" s="13">
+        <v>0.25600000000000001</v>
+      </c>
       <c r="D25" s="13">
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="E25" s="13">
         <v>0.21299999999999999</v>
       </c>
+      <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="I25" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K25" t="s">
         <v>120</v>
       </c>
+      <c r="L25">
+        <v>26</v>
+      </c>
       <c r="M25">
-        <v>26</v>
-      </c>
-      <c r="N25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13" t="s">
         <v>92</v>
       </c>
+      <c r="C26" s="13">
+        <v>0.22700000000000001</v>
+      </c>
       <c r="D26" s="13">
-        <v>0.22700000000000001</v>
+        <v>0.184</v>
       </c>
       <c r="E26" s="13">
-        <v>0.184</v>
+        <v>4</v>
       </c>
       <c r="F26" s="13">
-        <v>4</v>
+        <v>0.183</v>
       </c>
       <c r="G26" s="13">
-        <v>0.183</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H26" s="13">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I26" s="13">
         <v>4.1970000000000001</v>
       </c>
-      <c r="J26" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K26" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="I26" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" t="s">
         <v>120</v>
       </c>
+      <c r="L26">
+        <v>89</v>
+      </c>
       <c r="M26">
-        <v>89</v>
-      </c>
-      <c r="N26">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13" t="s">
+      <c r="B27" s="13" t="s">
         <v>93</v>
       </c>
+      <c r="C27" s="13">
+        <v>0.23499999999999999</v>
+      </c>
       <c r="D27" s="13">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="E27" s="13">
         <v>0.192</v>
       </c>
+      <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K27" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="I27" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K27" t="s">
         <v>120</v>
       </c>
+      <c r="L27">
+        <v>89</v>
+      </c>
       <c r="M27">
-        <v>89</v>
-      </c>
-      <c r="N27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13" t="s">
+      <c r="B28" s="13" t="s">
         <v>94</v>
       </c>
+      <c r="C28" s="13">
+        <v>0.216</v>
+      </c>
       <c r="D28" s="13">
-        <v>0.216</v>
-      </c>
-      <c r="E28" s="13">
         <v>0.17299999999999999</v>
       </c>
+      <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K28" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="I28" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K28" t="s">
         <v>120</v>
       </c>
+      <c r="L28">
+        <v>89</v>
+      </c>
       <c r="M28">
-        <v>89</v>
-      </c>
-      <c r="N28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="13" t="s">
         <v>95</v>
       </c>
+      <c r="C29" s="13">
+        <v>0.22600000000000001</v>
+      </c>
       <c r="D29" s="13">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="E29" s="13">
         <v>0.183</v>
       </c>
+      <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K29" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="I29" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K29" t="s">
         <v>120</v>
       </c>
+      <c r="L29">
+        <v>89</v>
+      </c>
       <c r="M29">
-        <v>89</v>
-      </c>
-      <c r="N29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13" t="s">
         <v>96</v>
       </c>
+      <c r="C30" s="13">
+        <v>0.247</v>
+      </c>
       <c r="D30" s="13">
-        <v>0.247</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="E30" s="13">
-        <v>0.20399999999999999</v>
+        <v>4</v>
       </c>
       <c r="F30" s="13">
-        <v>4</v>
+        <v>0.191</v>
       </c>
       <c r="G30" s="13">
-        <v>0.191</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H30" s="13">
-        <v>2.3E-2</v>
-      </c>
-      <c r="I30" s="13">
         <v>11.795</v>
       </c>
-      <c r="J30" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K30" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="I30" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K30" t="s">
         <v>121</v>
       </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
       <c r="M30">
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13" t="s">
+      <c r="B31" s="13" t="s">
         <v>97</v>
       </c>
+      <c r="C31" s="13">
+        <v>0.224</v>
+      </c>
       <c r="D31" s="13">
-        <v>0.224</v>
-      </c>
-      <c r="E31" s="13">
         <v>0.18099999999999999</v>
       </c>
+      <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K31" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L31" t="s">
+      <c r="I31" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K31" t="s">
         <v>121</v>
       </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
       <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13" t="s">
+      <c r="B32" s="13" t="s">
         <v>98</v>
       </c>
+      <c r="C32" s="13">
+        <v>0.25800000000000001</v>
+      </c>
       <c r="D32" s="13">
-        <v>0.25800000000000001</v>
-      </c>
-      <c r="E32" s="13">
         <v>0.215</v>
       </c>
+      <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K32" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L32" t="s">
+      <c r="I32" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K32" t="s">
         <v>121</v>
       </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
       <c r="M32">
-        <v>0</v>
-      </c>
-      <c r="N32">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13" t="s">
+      <c r="B33" s="13" t="s">
         <v>99</v>
       </c>
+      <c r="C33" s="13">
+        <v>0.20799999999999999</v>
+      </c>
       <c r="D33" s="13">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="E33" s="13">
         <v>0.16500000000000001</v>
       </c>
+      <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K33" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="I33" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K33" t="s">
         <v>121</v>
       </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
       <c r="M33">
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13" t="s">
         <v>100</v>
       </c>
+      <c r="C34" s="13">
+        <v>0.217</v>
+      </c>
       <c r="D34" s="13">
-        <v>0.217</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="E34" s="13">
+        <v>4</v>
+      </c>
+      <c r="F34" s="13">
         <v>0.17399999999999999</v>
       </c>
-      <c r="F34" s="13">
-        <v>4</v>
-      </c>
       <c r="G34" s="13">
-        <v>0.17399999999999999</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H34" s="13">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I34" s="13">
         <v>4.8659999999999997</v>
       </c>
-      <c r="J34" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K34" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L34" t="s">
+      <c r="I34" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K34" t="s">
         <v>121</v>
       </c>
+      <c r="L34">
+        <v>26</v>
+      </c>
       <c r="M34">
-        <v>26</v>
-      </c>
-      <c r="N34">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13" t="s">
+      <c r="B35" s="13" t="s">
         <v>101</v>
       </c>
+      <c r="C35" s="13">
+        <v>0.22800000000000001</v>
+      </c>
       <c r="D35" s="13">
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="E35" s="13">
         <v>0.185</v>
       </c>
+      <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K35" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L35" t="s">
+      <c r="I35" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K35" t="s">
         <v>121</v>
       </c>
+      <c r="L35">
+        <v>26</v>
+      </c>
       <c r="M35">
-        <v>26</v>
-      </c>
-      <c r="N35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13" t="s">
+      <c r="B36" s="13" t="s">
         <v>102</v>
       </c>
+      <c r="C36" s="13">
+        <v>0.216</v>
+      </c>
       <c r="D36" s="13">
-        <v>0.216</v>
-      </c>
-      <c r="E36" s="13">
         <v>0.17299999999999999</v>
       </c>
+      <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K36" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="I36" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K36" t="s">
         <v>121</v>
       </c>
+      <c r="L36">
+        <v>26</v>
+      </c>
       <c r="M36">
-        <v>26</v>
-      </c>
-      <c r="N36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13" t="s">
+      <c r="B37" s="13" t="s">
         <v>103</v>
       </c>
+      <c r="C37" s="13">
+        <v>0.20699999999999999</v>
+      </c>
       <c r="D37" s="13">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="E37" s="13">
         <v>0.16400000000000001</v>
       </c>
+      <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K37" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="I37" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K37" t="s">
         <v>121</v>
       </c>
+      <c r="L37">
+        <v>26</v>
+      </c>
       <c r="M37">
-        <v>26</v>
-      </c>
-      <c r="N37">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13" t="s">
         <v>104</v>
       </c>
+      <c r="C38" s="13">
+        <v>0.24099999999999999</v>
+      </c>
       <c r="D38" s="13">
-        <v>0.24099999999999999</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="E38" s="13">
-        <v>0.19800000000000001</v>
+        <v>4</v>
       </c>
       <c r="F38" s="13">
-        <v>4</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="G38" s="13">
-        <v>0.20100000000000001</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H38" s="13">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I38" s="13">
         <v>1.5149999999999999</v>
       </c>
-      <c r="J38" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K38" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="I38" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K38" t="s">
         <v>121</v>
       </c>
+      <c r="L38">
+        <v>89</v>
+      </c>
       <c r="M38">
-        <v>89</v>
-      </c>
-      <c r="N38">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13" t="s">
+      <c r="B39" s="13" t="s">
         <v>105</v>
       </c>
+      <c r="C39" s="13">
+        <v>0.24299999999999999</v>
+      </c>
       <c r="D39" s="13">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="E39" s="13">
         <v>0.2</v>
       </c>
+      <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K39" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L39" t="s">
+      <c r="I39" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K39" t="s">
         <v>121</v>
       </c>
+      <c r="L39">
+        <v>89</v>
+      </c>
       <c r="M39">
-        <v>89</v>
-      </c>
-      <c r="N39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13" t="s">
+      <c r="B40" s="13" t="s">
         <v>106</v>
       </c>
+      <c r="C40" s="13">
+        <v>0.246</v>
+      </c>
       <c r="D40" s="13">
-        <v>0.246</v>
-      </c>
-      <c r="E40" s="13">
         <v>0.20300000000000001</v>
       </c>
+      <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K40" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="I40" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K40" t="s">
         <v>121</v>
       </c>
+      <c r="L40">
+        <v>89</v>
+      </c>
       <c r="M40">
-        <v>89</v>
-      </c>
-      <c r="N40">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13" t="s">
+      <c r="B41" s="13" t="s">
         <v>107</v>
       </c>
+      <c r="C41" s="13">
+        <v>0.248</v>
+      </c>
       <c r="D41" s="13">
-        <v>0.248</v>
-      </c>
-      <c r="E41" s="13">
         <v>0.20499999999999999</v>
       </c>
+      <c r="E41" s="13"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K41" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L41" t="s">
+      <c r="I41" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J41" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K41" t="s">
         <v>121</v>
       </c>
+      <c r="L41">
+        <v>89</v>
+      </c>
       <c r="M41">
-        <v>89</v>
-      </c>
-      <c r="N41">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chris found that I didn't alter my dates between different beta gals. So, I fixed that in my code and thus the sensitivity values can now be calculated.
</commit_message>
<xml_diff>
--- a/myData/RAN 7-24-18 BETA GAL RAN11, RAN12, RAN13.xlsx
+++ b/myData/RAN 7-24-18 BETA GAL RAN11, RAN12, RAN13.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\royam\Documents\RpoSResearch\betaGal-analysis\myData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\Documents\betaGal-analysis\myData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6CF3C6-5169-4E85-BCC4-D10D3ABF1E9F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22992" windowHeight="13860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="122">
   <si>
     <t>A</t>
   </si>
@@ -393,7 +392,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -931,16 +930,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -979,7 +978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1059,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1179,7 +1178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1248,7 +1247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>16</v>
       </c>
@@ -1275,7 +1274,7 @@
         <v>-1.8455749075014E+16</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
@@ -1292,7 +1291,7 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
@@ -1309,7 +1308,7 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
@@ -1326,7 +1325,7 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>21</v>
       </c>
@@ -1353,7 +1352,7 @@
         <v>21.753</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13" t="s">
@@ -1370,7 +1369,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
@@ -1387,7 +1386,7 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13" t="s">
@@ -1404,7 +1403,7 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>26</v>
       </c>
@@ -1431,7 +1430,7 @@
         <v>5.3369999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13" t="s">
@@ -1448,7 +1447,7 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13" t="s">
@@ -1465,7 +1464,7 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13" t="s">
@@ -1482,7 +1481,7 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>31</v>
       </c>
@@ -1509,7 +1508,7 @@
         <v>3.5870000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13" t="s">
@@ -1526,7 +1525,7 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13" t="s">
@@ -1543,7 +1542,7 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13" t="s">
@@ -1560,7 +1559,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>36</v>
       </c>
@@ -1587,7 +1586,7 @@
         <v>5.65</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13" t="s">
@@ -1604,7 +1603,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13" t="s">
@@ -1621,7 +1620,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13" t="s">
@@ -1638,7 +1637,7 @@
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>41</v>
       </c>
@@ -1665,7 +1664,7 @@
         <v>3.9990000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13" t="s">
@@ -1682,7 +1681,7 @@
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13" t="s">
@@ -1699,7 +1698,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13" t="s">
@@ -1716,7 +1715,7 @@
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>46</v>
       </c>
@@ -1743,7 +1742,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13" t="s">
@@ -1760,7 +1759,7 @@
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13" t="s">
@@ -1777,7 +1776,7 @@
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13" t="s">
@@ -1794,7 +1793,7 @@
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
         <v>51</v>
       </c>
@@ -1821,7 +1820,7 @@
         <v>24.248000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13" t="s">
@@ -1838,7 +1837,7 @@
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13" t="s">
@@ -1855,7 +1854,7 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13" t="s">
@@ -1872,7 +1871,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
         <v>56</v>
       </c>
@@ -1899,7 +1898,7 @@
         <v>8.3149999999999995</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13" t="s">
@@ -1916,7 +1915,7 @@
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13" t="s">
@@ -1933,7 +1932,7 @@
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13" t="s">
@@ -1950,7 +1949,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
         <v>61</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>14.694000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13" t="s">
@@ -1994,7 +1993,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13" t="s">
@@ -2011,7 +2010,7 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13" t="s">
@@ -2028,7 +2027,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="2">
         <v>1</v>
@@ -2067,7 +2066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
@@ -2087,7 +2086,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>3</v>
       </c>
@@ -2127,7 +2126,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>4</v>
       </c>
@@ -2147,7 +2146,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
@@ -2187,7 +2186,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>6</v>
       </c>
@@ -2227,7 +2226,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>7</v>
       </c>
@@ -2267,7 +2266,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>8</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>9</v>
       </c>
@@ -2336,7 +2335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
         <v>16</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13" t="s">
@@ -2380,7 +2379,7 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13" t="s">
@@ -2397,7 +2396,7 @@
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13" t="s">
@@ -2414,7 +2413,7 @@
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
         <v>21</v>
       </c>
@@ -2441,7 +2440,7 @@
         <v>11.358000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13" t="s">
@@ -2458,7 +2457,7 @@
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13" t="s">
@@ -2475,7 +2474,7 @@
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13" t="s">
@@ -2492,7 +2491,7 @@
       <c r="H71" s="13"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="13" t="s">
         <v>26</v>
       </c>
@@ -2519,7 +2518,7 @@
         <v>4.7960000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13" t="s">
@@ -2536,7 +2535,7 @@
       <c r="H73" s="13"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13" t="s">
@@ -2553,7 +2552,7 @@
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13" t="s">
@@ -2570,7 +2569,7 @@
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="13" t="s">
         <v>31</v>
       </c>
@@ -2597,7 +2596,7 @@
         <v>7.17</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13" t="s">
@@ -2614,7 +2613,7 @@
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13" t="s">
@@ -2631,7 +2630,7 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13" t="s">
@@ -2648,7 +2647,7 @@
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="13" t="s">
         <v>36</v>
       </c>
@@ -2675,7 +2674,7 @@
         <v>6.06</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13" t="s">
@@ -2692,7 +2691,7 @@
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13" t="s">
@@ -2709,7 +2708,7 @@
       <c r="H82" s="13"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13" t="s">
@@ -2726,7 +2725,7 @@
       <c r="H83" s="13"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="13" t="s">
         <v>41</v>
       </c>
@@ -2753,7 +2752,7 @@
         <v>13.507999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13" t="s">
@@ -2770,7 +2769,7 @@
       <c r="H85" s="13"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13" t="s">
@@ -2787,7 +2786,7 @@
       <c r="H86" s="13"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13" t="s">
@@ -2804,7 +2803,7 @@
       <c r="H87" s="13"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="13" t="s">
         <v>46</v>
       </c>
@@ -2831,7 +2830,7 @@
         <v>4.1970000000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13" t="s">
@@ -2848,7 +2847,7 @@
       <c r="H89" s="13"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13" t="s">
@@ -2865,7 +2864,7 @@
       <c r="H90" s="13"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13" t="s">
@@ -2882,7 +2881,7 @@
       <c r="H91" s="13"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="13" t="s">
         <v>51</v>
       </c>
@@ -2909,7 +2908,7 @@
         <v>11.795</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13" t="s">
@@ -2926,7 +2925,7 @@
       <c r="H93" s="13"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13" t="s">
@@ -2943,7 +2942,7 @@
       <c r="H94" s="13"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13" t="s">
@@ -2960,7 +2959,7 @@
       <c r="H95" s="13"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="13" t="s">
         <v>56</v>
       </c>
@@ -2987,7 +2986,7 @@
         <v>4.8659999999999997</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="13" t="s">
@@ -3004,7 +3003,7 @@
       <c r="H97" s="13"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="C98" s="13" t="s">
@@ -3021,7 +3020,7 @@
       <c r="H98" s="13"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="C99" s="13" t="s">
@@ -3038,7 +3037,7 @@
       <c r="H99" s="13"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="13" t="s">
         <v>61</v>
       </c>
@@ -3065,7 +3064,7 @@
         <v>1.5149999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="13" t="s">
@@ -3082,7 +3081,7 @@
       <c r="H101" s="13"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="13"/>
       <c r="B102" s="13"/>
       <c r="C102" s="13" t="s">
@@ -3099,7 +3098,7 @@
       <c r="H102" s="13"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="13"/>
       <c r="B103" s="13"/>
       <c r="C103" s="13" t="s">
@@ -3123,102 +3122,105 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="11" max="11" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.26953125" customWidth="1"/>
+    <col min="14" max="14" width="13.08984375" customWidth="1"/>
+    <col min="15" max="15" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2">
+      <c r="C1" s="2">
         <v>420</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E1" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="I1" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="J1" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="P1" s="17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="13" t="s">
         <v>17</v>
       </c>
+      <c r="C2" s="13">
+        <v>5.1999999999999998E-2</v>
+      </c>
       <c r="D2" s="13">
-        <v>5.1999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="E2" s="13">
+        <v>4</v>
+      </c>
+      <c r="F2" s="13">
         <v>0</v>
-      </c>
-      <c r="F2" s="13">
-        <v>4</v>
       </c>
       <c r="G2" s="13">
         <v>0</v>
       </c>
       <c r="H2" s="13">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13">
         <v>-1.8455749075014E+16</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I2" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" t="s">
         <v>117</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>119</v>
       </c>
       <c r="M2" s="20" t="s">
         <v>119</v>
@@ -3229,34 +3231,33 @@
       <c r="O2" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="P2" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
+      <c r="C3" s="13">
+        <v>5.1999999999999998E-2</v>
+      </c>
       <c r="D3" s="13">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="E3" s="13">
         <v>0</v>
       </c>
+      <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="I3" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" t="s">
         <v>117</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>119</v>
       </c>
       <c r="M3" s="20" t="s">
         <v>119</v>
@@ -3267,34 +3268,33 @@
       <c r="O3" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="P3" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
+      <c r="C4" s="13">
+        <v>5.1999999999999998E-2</v>
+      </c>
       <c r="D4" s="13">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="E4" s="13">
         <v>0</v>
       </c>
+      <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="I4" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" t="s">
         <v>117</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>119</v>
       </c>
       <c r="M4" s="20" t="s">
         <v>119</v>
@@ -3305,34 +3305,33 @@
       <c r="O4" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="P4" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="13" t="s">
         <v>20</v>
       </c>
+      <c r="C5" s="13">
+        <v>5.1999999999999998E-2</v>
+      </c>
       <c r="D5" s="13">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="E5" s="13">
         <v>0</v>
       </c>
+      <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="I5" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" t="s">
         <v>117</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>119</v>
       </c>
       <c r="M5" s="20" t="s">
         <v>119</v>
@@ -3343,1465 +3342,1426 @@
       <c r="O5" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="P5" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="13" t="s">
         <v>22</v>
       </c>
+      <c r="C6" s="13">
+        <v>6.6000000000000003E-2</v>
+      </c>
       <c r="D6" s="13">
-        <v>6.6000000000000003E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="E6" s="13">
-        <v>1.4E-2</v>
+        <v>4</v>
       </c>
       <c r="F6" s="13">
-        <v>4</v>
+        <v>1.6E-2</v>
       </c>
       <c r="G6" s="13">
-        <v>1.6E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H6" s="13">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="I6" s="13">
         <v>21.753</v>
       </c>
-      <c r="J6" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="I6" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" t="s">
         <v>118</v>
       </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
       <c r="M6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N6">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O6">
-        <v>0.1</v>
-      </c>
-      <c r="P6">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="C7" s="13">
+        <v>6.7000000000000004E-2</v>
+      </c>
       <c r="D7" s="13">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="E7" s="13">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="I7" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" t="s">
         <v>118</v>
       </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
       <c r="M7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N7">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O7">
-        <v>0.1</v>
-      </c>
-      <c r="P7">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="13" t="s">
         <v>24</v>
       </c>
+      <c r="C8" s="13">
+        <v>7.3999999999999996E-2</v>
+      </c>
       <c r="D8" s="13">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="E8" s="13">
         <v>2.1999999999999999E-2</v>
       </c>
+      <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="I8" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" t="s">
         <v>118</v>
       </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
       <c r="M8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N8">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O8">
-        <v>0.1</v>
-      </c>
-      <c r="P8">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="13" t="s">
         <v>25</v>
       </c>
+      <c r="C9" s="13">
+        <v>6.7000000000000004E-2</v>
+      </c>
       <c r="D9" s="13">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="E9" s="13">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="I9" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" t="s">
         <v>118</v>
       </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
       <c r="M9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N9">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O9">
-        <v>0.1</v>
-      </c>
-      <c r="P9">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="13" t="s">
         <v>27</v>
       </c>
+      <c r="C10" s="13">
+        <v>0.14099999999999999</v>
+      </c>
       <c r="D10" s="13">
-        <v>0.14099999999999999</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E10" s="13">
-        <v>8.8999999999999996E-2</v>
+        <v>4</v>
       </c>
       <c r="F10" s="13">
-        <v>4</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="G10" s="13">
-        <v>9.1999999999999998E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H10" s="13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I10" s="13">
         <v>5.3369999999999997</v>
       </c>
-      <c r="J10" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="I10" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K10" t="s">
         <v>118</v>
       </c>
+      <c r="L10">
+        <v>26</v>
+      </c>
       <c r="M10">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="N10">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O10">
-        <v>0.1</v>
-      </c>
-      <c r="P10">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="13" t="s">
         <v>28</v>
       </c>
+      <c r="C11" s="13">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="D11" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E11" s="13">
         <v>8.7999999999999995E-2</v>
       </c>
+      <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="I11" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K11" t="s">
         <v>118</v>
       </c>
+      <c r="L11">
+        <v>26</v>
+      </c>
       <c r="M11">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="N11">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O11">
-        <v>0.1</v>
-      </c>
-      <c r="P11">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="13" t="s">
         <v>29</v>
       </c>
+      <c r="C12" s="13">
+        <v>0.14399999999999999</v>
+      </c>
       <c r="D12" s="13">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="E12" s="13">
         <v>9.1999999999999998E-2</v>
       </c>
+      <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="I12" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K12" t="s">
         <v>118</v>
       </c>
+      <c r="L12">
+        <v>26</v>
+      </c>
       <c r="M12">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="N12">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O12">
-        <v>0.1</v>
-      </c>
-      <c r="P12">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="13" t="s">
         <v>30</v>
       </c>
+      <c r="C13" s="13">
+        <v>0.151</v>
+      </c>
       <c r="D13" s="13">
-        <v>0.151</v>
-      </c>
-      <c r="E13" s="13">
         <v>9.9000000000000005E-2</v>
       </c>
+      <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="I13" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" t="s">
         <v>118</v>
       </c>
+      <c r="L13">
+        <v>26</v>
+      </c>
       <c r="M13">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="N13">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O13">
-        <v>0.1</v>
-      </c>
-      <c r="P13">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="13" t="s">
         <v>32</v>
       </c>
+      <c r="C14" s="13">
+        <v>0.41599999999999998</v>
+      </c>
       <c r="D14" s="13">
-        <v>0.41599999999999998</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="E14" s="13">
-        <v>0.36399999999999999</v>
+        <v>4</v>
       </c>
       <c r="F14" s="13">
-        <v>4</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="G14" s="13">
-        <v>0.34799999999999998</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H14" s="13">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="I14" s="13">
         <v>3.5870000000000002</v>
       </c>
-      <c r="J14" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="I14" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K14" t="s">
         <v>118</v>
       </c>
+      <c r="L14">
+        <v>89</v>
+      </c>
       <c r="M14">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="N14">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O14">
-        <v>0.1</v>
-      </c>
-      <c r="P14">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="13" t="s">
         <v>33</v>
       </c>
+      <c r="C15" s="13">
+        <v>0.40100000000000002</v>
+      </c>
       <c r="D15" s="13">
-        <v>0.40100000000000002</v>
-      </c>
-      <c r="E15" s="13">
         <v>0.34899999999999998</v>
       </c>
+      <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="I15" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" t="s">
         <v>118</v>
       </c>
+      <c r="L15">
+        <v>89</v>
+      </c>
       <c r="M15">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="N15">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O15">
-        <v>0.1</v>
-      </c>
-      <c r="P15">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="13" t="s">
         <v>34</v>
       </c>
+      <c r="C16" s="13">
+        <v>0.4</v>
+      </c>
       <c r="D16" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="E16" s="13">
         <v>0.34799999999999998</v>
       </c>
+      <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="I16" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" t="s">
         <v>118</v>
       </c>
+      <c r="L16">
+        <v>89</v>
+      </c>
       <c r="M16">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="N16">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O16">
-        <v>0.1</v>
-      </c>
-      <c r="P16">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="13" t="s">
         <v>35</v>
       </c>
+      <c r="C17" s="13">
+        <v>0.38600000000000001</v>
+      </c>
       <c r="D17" s="13">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="E17" s="13">
         <v>0.33300000000000002</v>
       </c>
+      <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="I17" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K17" t="s">
         <v>118</v>
       </c>
+      <c r="L17">
+        <v>89</v>
+      </c>
       <c r="M17">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="N17">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O17">
-        <v>0.1</v>
-      </c>
-      <c r="P17">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13" t="s">
+      <c r="B18" s="13" t="s">
         <v>37</v>
       </c>
+      <c r="C18" s="13">
+        <v>0.151</v>
+      </c>
       <c r="D18" s="13">
-        <v>0.151</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="E18" s="13">
-        <v>9.9000000000000005E-2</v>
+        <v>4</v>
       </c>
       <c r="F18" s="13">
-        <v>4</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="G18" s="13">
-        <v>9.1999999999999998E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H18" s="13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I18" s="13">
         <v>5.65</v>
       </c>
-      <c r="J18" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K18" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="I18" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" t="s">
         <v>120</v>
       </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
       <c r="M18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N18">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O18">
-        <v>0.1</v>
-      </c>
-      <c r="P18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="13" t="s">
         <v>38</v>
       </c>
+      <c r="C19" s="13">
+        <v>0.14299999999999999</v>
+      </c>
       <c r="D19" s="13">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="E19" s="13">
         <v>9.0999999999999998E-2</v>
       </c>
+      <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="I19" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K19" t="s">
         <v>120</v>
       </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
       <c r="M19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N19">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O19">
-        <v>0.1</v>
-      </c>
-      <c r="P19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="C20" s="13">
+        <v>0.14399999999999999</v>
+      </c>
       <c r="D20" s="13">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="E20" s="13">
         <v>9.1999999999999998E-2</v>
       </c>
+      <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="I20" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K20" t="s">
         <v>120</v>
       </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
       <c r="M20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N20">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O20">
-        <v>0.1</v>
-      </c>
-      <c r="P20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="13" t="s">
         <v>40</v>
       </c>
+      <c r="C21" s="13">
+        <v>0.13800000000000001</v>
+      </c>
       <c r="D21" s="13">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="E21" s="13">
         <v>8.5999999999999993E-2</v>
       </c>
+      <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="I21" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K21" t="s">
         <v>120</v>
       </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
       <c r="M21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N21">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O21">
-        <v>0.1</v>
-      </c>
-      <c r="P21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13" t="s">
+      <c r="B22" s="13" t="s">
         <v>42</v>
       </c>
+      <c r="C22" s="13">
+        <v>0.28100000000000003</v>
+      </c>
       <c r="D22" s="13">
-        <v>0.28100000000000003</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="E22" s="13">
-        <v>0.22900000000000001</v>
+        <v>4</v>
       </c>
       <c r="F22" s="13">
-        <v>4</v>
+        <v>0.219</v>
       </c>
       <c r="G22" s="13">
-        <v>0.219</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H22" s="13">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I22" s="13">
         <v>3.9990000000000001</v>
       </c>
-      <c r="J22" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="I22" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" t="s">
         <v>120</v>
       </c>
+      <c r="L22">
+        <v>26</v>
+      </c>
       <c r="M22">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="N22">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O22">
-        <v>0.1</v>
-      </c>
-      <c r="P22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="13" t="s">
         <v>43</v>
       </c>
+      <c r="C23" s="13">
+        <v>0.27600000000000002</v>
+      </c>
       <c r="D23" s="13">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="E23" s="13">
         <v>0.224</v>
       </c>
+      <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="I23" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K23" t="s">
         <v>120</v>
       </c>
+      <c r="L23">
+        <v>26</v>
+      </c>
       <c r="M23">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="N23">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O23">
-        <v>0.1</v>
-      </c>
-      <c r="P23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="13" t="s">
         <v>44</v>
       </c>
+      <c r="C24" s="13">
+        <v>0.26600000000000001</v>
+      </c>
       <c r="D24" s="13">
-        <v>0.26600000000000001</v>
-      </c>
-      <c r="E24" s="13">
         <v>0.214</v>
       </c>
+      <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="I24" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K24" t="s">
         <v>120</v>
       </c>
+      <c r="L24">
+        <v>26</v>
+      </c>
       <c r="M24">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="N24">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O24">
-        <v>0.1</v>
-      </c>
-      <c r="P24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="13" t="s">
         <v>45</v>
       </c>
+      <c r="C25" s="13">
+        <v>0.26200000000000001</v>
+      </c>
       <c r="D25" s="13">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="E25" s="13">
         <v>0.21</v>
       </c>
+      <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="I25" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K25" t="s">
         <v>120</v>
       </c>
+      <c r="L25">
+        <v>26</v>
+      </c>
       <c r="M25">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="N25">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O25">
-        <v>0.1</v>
-      </c>
-      <c r="P25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13" t="s">
+      <c r="B26" s="13" t="s">
         <v>47</v>
       </c>
+      <c r="C26" s="13">
+        <v>0.26</v>
+      </c>
       <c r="D26" s="13">
-        <v>0.26</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="E26" s="13">
-        <v>0.20699999999999999</v>
+        <v>4</v>
       </c>
       <c r="F26" s="13">
-        <v>4</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="G26" s="13">
-        <v>0.20100000000000001</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H26" s="13">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="I26" s="13">
         <v>2.93</v>
       </c>
-      <c r="J26" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K26" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="I26" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" t="s">
         <v>120</v>
       </c>
+      <c r="L26">
+        <v>89</v>
+      </c>
       <c r="M26">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="N26">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O26">
-        <v>0.1</v>
-      </c>
-      <c r="P26">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13" t="s">
+      <c r="B27" s="13" t="s">
         <v>48</v>
       </c>
+      <c r="C27" s="13">
+        <v>0.25600000000000001</v>
+      </c>
       <c r="D27" s="13">
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="E27" s="13">
         <v>0.20399999999999999</v>
       </c>
+      <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K27" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="I27" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K27" t="s">
         <v>120</v>
       </c>
+      <c r="L27">
+        <v>89</v>
+      </c>
       <c r="M27">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="N27">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O27">
-        <v>0.1</v>
-      </c>
-      <c r="P27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13" t="s">
+      <c r="B28" s="13" t="s">
         <v>49</v>
       </c>
+      <c r="C28" s="13">
+        <v>0.253</v>
+      </c>
       <c r="D28" s="13">
-        <v>0.253</v>
-      </c>
-      <c r="E28" s="13">
         <v>0.20100000000000001</v>
       </c>
+      <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K28" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="I28" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K28" t="s">
         <v>120</v>
       </c>
+      <c r="L28">
+        <v>89</v>
+      </c>
       <c r="M28">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="N28">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O28">
-        <v>0.1</v>
-      </c>
-      <c r="P28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="13" t="s">
         <v>50</v>
       </c>
+      <c r="C29" s="13">
+        <v>0.246</v>
+      </c>
       <c r="D29" s="13">
-        <v>0.246</v>
-      </c>
-      <c r="E29" s="13">
         <v>0.19400000000000001</v>
       </c>
+      <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K29" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="I29" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K29" t="s">
         <v>120</v>
       </c>
+      <c r="L29">
+        <v>89</v>
+      </c>
       <c r="M29">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="N29">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="O29">
-        <v>0.1</v>
-      </c>
-      <c r="P29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13" t="s">
+      <c r="B30" s="13" t="s">
         <v>52</v>
       </c>
+      <c r="C30" s="13">
+        <v>5.5E-2</v>
+      </c>
       <c r="D30" s="13">
-        <v>5.5E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E30" s="13">
+        <v>4</v>
+      </c>
+      <c r="F30" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G30" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="H30" s="13">
+        <v>24.248000000000001</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K30" t="s">
+        <v>121</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>100</v>
+      </c>
+      <c r="N30">
+        <v>0.1</v>
+      </c>
+      <c r="O30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="D31" s="13">
         <v>2E-3</v>
       </c>
-      <c r="F30" s="13">
-        <v>4</v>
-      </c>
-      <c r="G30" s="13">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H30" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="I30" s="13">
-        <v>24.248000000000001</v>
-      </c>
-      <c r="J30" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K30" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L30" t="s">
-        <v>121</v>
-      </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <v>100</v>
-      </c>
-      <c r="O30">
-        <v>0.1</v>
-      </c>
-      <c r="P30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="13">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="E31" s="13">
-        <v>2E-3</v>
-      </c>
+      <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K31" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L31" t="s">
+      <c r="I31" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K31" t="s">
         <v>121</v>
       </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
       <c r="M31">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N31">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O31">
-        <v>0.1</v>
-      </c>
-      <c r="P31">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13" t="s">
+      <c r="B32" s="13" t="s">
         <v>54</v>
       </c>
+      <c r="C32" s="13">
+        <v>5.6000000000000001E-2</v>
+      </c>
       <c r="D32" s="13">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="E32" s="13">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K32" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L32" t="s">
+      <c r="I32" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K32" t="s">
         <v>121</v>
       </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
       <c r="M32">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N32">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O32">
-        <v>0.1</v>
-      </c>
-      <c r="P32">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13" t="s">
+      <c r="B33" s="13" t="s">
         <v>55</v>
       </c>
+      <c r="C33" s="13">
+        <v>5.6000000000000001E-2</v>
+      </c>
       <c r="D33" s="13">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="E33" s="13">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K33" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="I33" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K33" t="s">
         <v>121</v>
       </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
       <c r="M33">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N33">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O33">
-        <v>0.1</v>
-      </c>
-      <c r="P33">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13" t="s">
+      <c r="B34" s="13" t="s">
         <v>57</v>
       </c>
+      <c r="C34" s="13">
+        <v>0.08</v>
+      </c>
       <c r="D34" s="13">
-        <v>0.08</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="E34" s="13">
-        <v>2.8000000000000001E-2</v>
+        <v>4</v>
       </c>
       <c r="F34" s="13">
-        <v>4</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G34" s="13">
-        <v>2.5999999999999999E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="H34" s="13">
-        <v>2E-3</v>
-      </c>
-      <c r="I34" s="13">
         <v>8.3149999999999995</v>
       </c>
-      <c r="J34" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K34" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L34" t="s">
+      <c r="I34" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K34" t="s">
         <v>121</v>
       </c>
+      <c r="L34">
+        <v>26</v>
+      </c>
       <c r="M34">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="N34">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O34">
-        <v>0.1</v>
-      </c>
-      <c r="P34">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13" t="s">
+      <c r="B35" s="13" t="s">
         <v>58</v>
       </c>
+      <c r="C35" s="13">
+        <v>7.6999999999999999E-2</v>
+      </c>
       <c r="D35" s="13">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="E35" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K35" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L35" t="s">
+      <c r="I35" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K35" t="s">
         <v>121</v>
       </c>
+      <c r="L35">
+        <v>26</v>
+      </c>
       <c r="M35">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="N35">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O35">
-        <v>0.1</v>
-      </c>
-      <c r="P35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13" t="s">
+      <c r="B36" s="13" t="s">
         <v>59</v>
       </c>
+      <c r="C36" s="13">
+        <v>7.9000000000000001E-2</v>
+      </c>
       <c r="D36" s="13">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="E36" s="13">
         <v>2.7E-2</v>
       </c>
+      <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K36" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="I36" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K36" t="s">
         <v>121</v>
       </c>
+      <c r="L36">
+        <v>26</v>
+      </c>
       <c r="M36">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="N36">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O36">
-        <v>0.1</v>
-      </c>
-      <c r="P36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13" t="s">
+      <c r="B37" s="13" t="s">
         <v>60</v>
       </c>
+      <c r="C37" s="13">
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="D37" s="13">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E37" s="13">
         <v>2.3E-2</v>
       </c>
+      <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K37" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="I37" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K37" t="s">
         <v>121</v>
       </c>
+      <c r="L37">
+        <v>26</v>
+      </c>
       <c r="M37">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="N37">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O37">
-        <v>0.1</v>
-      </c>
-      <c r="P37">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13" t="s">
+      <c r="B38" s="13" t="s">
         <v>62</v>
       </c>
+      <c r="C38" s="13">
+        <v>0.79900000000000004</v>
+      </c>
       <c r="D38" s="13">
-        <v>0.79900000000000004</v>
+        <v>0.747</v>
       </c>
       <c r="E38" s="13">
-        <v>0.747</v>
+        <v>4</v>
       </c>
       <c r="F38" s="13">
-        <v>4</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="G38" s="13">
-        <v>0.66100000000000003</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="H38" s="13">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="I38" s="13">
         <v>14.694000000000001</v>
       </c>
-      <c r="J38" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K38" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="I38" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K38" t="s">
         <v>121</v>
       </c>
+      <c r="L38">
+        <v>89</v>
+      </c>
       <c r="M38">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="N38">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O38">
-        <v>0.1</v>
-      </c>
-      <c r="P38">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13" t="s">
+      <c r="B39" s="13" t="s">
         <v>63</v>
       </c>
+      <c r="C39" s="13">
+        <v>0.57699999999999996</v>
+      </c>
       <c r="D39" s="13">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="E39" s="13">
         <v>0.52500000000000002</v>
       </c>
+      <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K39" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L39" t="s">
+      <c r="I39" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K39" t="s">
         <v>121</v>
       </c>
+      <c r="L39">
+        <v>89</v>
+      </c>
       <c r="M39">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="N39">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O39">
-        <v>0.1</v>
-      </c>
-      <c r="P39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13" t="s">
+      <c r="B40" s="13" t="s">
         <v>64</v>
       </c>
+      <c r="C40" s="13">
+        <v>0.71499999999999997</v>
+      </c>
       <c r="D40" s="13">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="E40" s="13">
         <v>0.66200000000000003</v>
       </c>
+      <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K40" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="I40" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K40" t="s">
         <v>121</v>
       </c>
+      <c r="L40">
+        <v>89</v>
+      </c>
       <c r="M40">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="N40">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O40">
-        <v>0.1</v>
-      </c>
-      <c r="P40">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13" t="s">
+      <c r="B41" s="13" t="s">
         <v>65</v>
       </c>
+      <c r="C41" s="13">
+        <v>0.76200000000000001</v>
+      </c>
       <c r="D41" s="13">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="E41" s="13">
         <v>0.71</v>
       </c>
+      <c r="E41" s="13"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="K41" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L41" t="s">
+      <c r="I41" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J41" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K41" t="s">
         <v>121</v>
       </c>
+      <c r="L41">
+        <v>89</v>
+      </c>
       <c r="M41">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="N41">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="O41">
-        <v>0.1</v>
-      </c>
-      <c r="P41">
         <v>10</v>
       </c>
     </row>
@@ -4812,18 +4772,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="9.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>11</v>
@@ -4862,8 +4825,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="B2" s="13" t="s">
         <v>67</v>
       </c>
@@ -4901,7 +4866,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="13" t="s">
         <v>69</v>
@@ -4932,7 +4897,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
       <c r="B4" s="13" t="s">
         <v>70</v>
@@ -4963,7 +4928,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
       <c r="B5" s="13" t="s">
         <v>71</v>
@@ -4994,8 +4959,10 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="B6" s="13" t="s">
         <v>72</v>
       </c>
@@ -5033,7 +5000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="13" t="s">
         <v>73</v>
@@ -5064,7 +5031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="13" t="s">
         <v>74</v>
@@ -5095,7 +5062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="13" t="s">
         <v>75</v>
@@ -5126,8 +5093,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="B10" s="13" t="s">
         <v>76</v>
       </c>
@@ -5165,7 +5134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="13" t="s">
         <v>77</v>
@@ -5196,7 +5165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="13" t="s">
         <v>78</v>
@@ -5227,7 +5196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
       <c r="B13" s="13" t="s">
         <v>79</v>
@@ -5258,8 +5227,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="B14" s="13" t="s">
         <v>80</v>
       </c>
@@ -5297,7 +5268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="13" t="s">
         <v>81</v>
@@ -5328,7 +5299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="13" t="s">
         <v>82</v>
@@ -5359,7 +5330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="13" t="s">
         <v>83</v>
@@ -5390,8 +5361,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="B18" s="13" t="s">
         <v>84</v>
       </c>
@@ -5429,7 +5402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="13" t="s">
         <v>85</v>
@@ -5460,7 +5433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="13" t="s">
         <v>86</v>
@@ -5491,7 +5464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="13" t="s">
         <v>87</v>
@@ -5522,8 +5495,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="B22" s="13" t="s">
         <v>88</v>
       </c>
@@ -5561,7 +5536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="13" t="s">
         <v>89</v>
@@ -5592,7 +5567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="13" t="s">
         <v>90</v>
@@ -5623,7 +5598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
       <c r="B25" s="13" t="s">
         <v>91</v>
@@ -5654,8 +5629,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="B26" s="13" t="s">
         <v>92</v>
       </c>
@@ -5693,7 +5670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="13" t="s">
         <v>93</v>
@@ -5724,7 +5701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="13" t="s">
         <v>94</v>
@@ -5755,7 +5732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13" t="s">
         <v>95</v>
@@ -5786,8 +5763,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="B30" s="13" t="s">
         <v>96</v>
       </c>
@@ -5825,7 +5804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13" t="s">
         <v>97</v>
@@ -5856,7 +5835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="13" t="s">
         <v>98</v>
@@ -5887,7 +5866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="13" t="s">
         <v>99</v>
@@ -5918,8 +5897,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B34" s="13" t="s">
         <v>100</v>
       </c>
@@ -5957,7 +5938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13" t="s">
         <v>101</v>
@@ -5988,7 +5969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="13" t="s">
         <v>102</v>
@@ -6019,7 +6000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="13" t="s">
         <v>103</v>
@@ -6050,8 +6031,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="B38" s="13" t="s">
         <v>104</v>
       </c>
@@ -6089,7 +6072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="13" t="s">
         <v>105</v>
@@ -6120,7 +6103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
       <c r="B40" s="13" t="s">
         <v>106</v>
@@ -6151,7 +6134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="13" t="s">
         <v>107</v>

</xml_diff>